<commit_message>
Complete Cover Sheet and removed use for tblPurchaseOrder_Exceptions
</commit_message>
<xml_diff>
--- a/LW_Web/_Templates/_Template - VacancyCoverSheet.xlsx
+++ b/LW_Web/_Templates/_Template - VacancyCoverSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Source\Repos\lemlewolff\LW_Web\_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F1E5FA-05EE-4A69-ADCD-DDC8B9CDE5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81969476-268B-402F-BA93-3193C4F0A335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2328" yWindow="456" windowWidth="20088" windowHeight="11496" xr2:uid="{84E44342-FB58-4183-99AA-46E39B299C64}"/>
+    <workbookView xWindow="4296" yWindow="348" windowWidth="17076" windowHeight="11568" xr2:uid="{84E44342-FB58-4183-99AA-46E39B299C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Vacancy Proposal Cover Sheet</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>New Rent - 2yr:</t>
+  </si>
+  <si>
+    <t>PROPOSED COSTS</t>
+  </si>
+  <si>
+    <t>TOTAL COST:</t>
+  </si>
+  <si>
+    <t>Agent Signature:</t>
+  </si>
+  <si>
+    <t>A/E Signature:</t>
+  </si>
+  <si>
+    <t>Joe Z. Signature:</t>
+  </si>
+  <si>
+    <t>WO Numbers</t>
   </si>
 </sst>
 </file>
@@ -86,9 +104,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +160,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -151,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -174,12 +207,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -206,11 +294,50 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -550,26 +677,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -583,7 +712,8 @@
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -599,6 +729,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="4"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -613,7 +744,7 @@
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="10"/>
     </row>
     <row r="15" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -622,43 +753,147 @@
       </c>
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="5"/>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="19"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="16"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="19"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="16"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="19"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="16"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="19"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="16"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="19"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="16"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="19"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="16"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="19"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="16"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="19"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="19"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="16"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="19"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="16"/>
+    </row>
+    <row r="38" spans="1:3" ht="3.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="14">
+        <f>SUM(B26:B37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+    </row>
+    <row r="41" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+    </row>
+    <row r="42" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="88" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>